<commit_message>
typo in model map
</commit_message>
<xml_diff>
--- a/timestamps.xlsx
+++ b/timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Uni CS\Graduate\COMSE6998_012 - Practical DL\Project\distributed-ml-prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31EB106-6864-48D2-A3C8-167D9309598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A91201F-0001-4D6F-9656-285DC664A934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{816BF27E-68D6-4FE0-A21F-F97AED8A31BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>k</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Dec 10, 2021, 6:20:02 PM</t>
+  </si>
+  <si>
+    <t>model_2021-12-10003229.029417</t>
   </si>
 </sst>
 </file>
@@ -231,14 +234,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -558,7 +561,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +643,7 @@
         <v>132.19999999999999</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>0.25</v>
       </c>
       <c r="L2" s="2"/>
@@ -752,7 +755,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
@@ -925,17 +928,17 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -979,7 +982,7 @@
       <c r="B14" s="2">
         <v>3</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -991,7 +994,7 @@
       <c r="F14" s="2">
         <v>5</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <v>19</v>
       </c>
       <c r="H14" s="2">
@@ -1003,7 +1006,7 @@
         <v>103.4</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="K14" s="11">
+      <c r="K14" s="10">
         <v>1</v>
       </c>
       <c r="L14" s="2"/>
@@ -1015,7 +1018,7 @@
       <c r="B15" s="2">
         <v>5</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="1" t="s">

</xml_diff>